<commit_message>
Updated version of initial driver
Added initial support for self/soft calibration of current & power
offsets (not complete or correct yet)
Initial support for additional accuracy with inclusion of RMS register
data (untested)
Added API's to dynamically change the LIVE & NEUTRAL Gain, enabling
range selection.
Added compile time option to in/exclude support for the NEUTRAL line
</commit_message>
<xml_diff>
--- a/m90e26_calibrate.xlsx
+++ b/m90e26_calibrate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\devs\ws\z-components\devices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\devs\ws\z-components\devices\m90e26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{892822A4-EC2B-4E9F-A162-E53CB9BC09C6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14C64AB1-D980-4A1C-B5A4-2B01B10E021A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12480" xr2:uid="{FE178CC8-A0CF-4137-A708-A44CFB898DD1}"/>
   </bookViews>
@@ -24,6 +24,8 @@
     <definedName name="Cur_meaL">Sheet1!$C$39</definedName>
     <definedName name="Gl">Sheet1!$C$5</definedName>
     <definedName name="Ib">Sheet1!$C$4</definedName>
+    <definedName name="Kn">Sheet1!$C$26</definedName>
+    <definedName name="Ks">Sheet1!$C$24</definedName>
     <definedName name="Lgain">Sheet1!$C$14</definedName>
     <definedName name="Lphi">Sheet1!$C$20</definedName>
     <definedName name="Lratio">Sheet1!$C$13</definedName>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Reference Voltage</t>
   </si>
@@ -124,9 +126,6 @@
     <t>---------------- L Line Calibration Angle (Pf must be 0.5L, Freq=50Hz current=Ib)</t>
   </si>
   <si>
-    <t>----------------- L Line Gain Calibration (PF must be 1.0,m current = Ib)</t>
-  </si>
-  <si>
     <t>Calibration Bench Error Ratio</t>
   </si>
   <si>
@@ -151,9 +150,6 @@
     <t>Measured/displayed voltage</t>
   </si>
   <si>
-    <t>Vgain</t>
-  </si>
-  <si>
     <t>Vol_mea</t>
   </si>
   <si>
@@ -185,6 +181,69 @@
   </si>
   <si>
     <t>Cur_defL</t>
+  </si>
+  <si>
+    <t>----------------- L Line Gain Calibration (PF must be 1.0,current = Ib)</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Shown</t>
+  </si>
+  <si>
+    <t>---------------- Startup/NoLoad, Power/Current Threshold</t>
+  </si>
+  <si>
+    <t>Ks</t>
+  </si>
+  <si>
+    <t>Kn</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>PStartTh</t>
+  </si>
+  <si>
+    <t>pNolTh</t>
+  </si>
+  <si>
+    <t>7A13</t>
+  </si>
+  <si>
+    <t>6720</t>
+  </si>
+  <si>
+    <t>6C50</t>
+  </si>
+  <si>
+    <t>-----------------------N Line Current RMS Gain</t>
+  </si>
+  <si>
+    <t>IgainN Register Default Value</t>
+  </si>
+  <si>
+    <t>IgainN Actual Register Value</t>
+  </si>
+  <si>
+    <t>Cur_defN</t>
+  </si>
+  <si>
+    <t>Cur_meaN</t>
+  </si>
+  <si>
+    <t>I_GAIN_L</t>
+  </si>
+  <si>
+    <t>I_GAIN_N</t>
+  </si>
+  <si>
+    <t>V_GAIN</t>
+  </si>
+  <si>
+    <t>0282</t>
   </si>
 </sst>
 </file>
@@ -234,12 +293,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165B2767-E119-42EF-B23D-1E7D6222F4D5}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +633,7 @@
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -582,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -596,7 +661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -610,7 +675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -624,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -635,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -649,7 +714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -663,7 +728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -671,7 +736,7 @@
         <v>838860800</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -684,27 +749,40 @@
         <v>0006EDD5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="2">
-        <v>-0.13780000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <f>(F12-E12)/E12</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F12">
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -713,10 +791,10 @@
       </c>
       <c r="C13" s="3">
         <f>-_e/(1+_e)</f>
-        <v>0.15982370679656693</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -725,46 +803,59 @@
       </c>
       <c r="C14" s="4">
         <f>IF(Lratio&gt;=0,Lratio*2^15,2^16+(Lratio*2^15))</f>
-        <v>5237.1032243099053</v>
+        <v>0</v>
       </c>
       <c r="D14" s="3" t="str">
         <f>DEC2HEX(INT(C14),8)</f>
-        <v>00001475</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2">
+        <f>(F17-E17)/E17</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="2">
-        <v>9.4999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <f>-_el*(180/SQRT(3)/PI())</f>
-        <v>-0.31425747039042151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -772,141 +863,250 @@
         <v>3763.74</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
       </c>
       <c r="C20" s="4">
         <f>_el*C19</f>
-        <v>35.75553</v>
+        <v>0</v>
       </c>
       <c r="D20" s="3" t="str">
         <f>DEC2HEX(INT(C20),8)</f>
-        <v>00000023</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>93.206755599999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25">
+        <f>C23*Gl*Vl*Vu*Ks</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
+        <f>C23*Gl*Vl*Vu*Kn</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32">
-        <f>HEX2DEC(6720)</f>
+        <v>32</v>
+      </c>
+      <c r="C32" s="3">
+        <f>HEX2DEC(D32)</f>
         <v>26400</v>
       </c>
-      <c r="D32" t="s">
-        <v>9</v>
+      <c r="D32" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33">
-        <f>HEX2DEC("6C50")/100</f>
+        <v>34</v>
+      </c>
+      <c r="C33" s="3">
+        <f>HEX2DEC(D33)/100</f>
         <v>277.27999999999997</v>
       </c>
-      <c r="D33" t="s">
-        <v>9</v>
+      <c r="D33" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34">
-        <v>220.7</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
+      <c r="B35" t="s">
+        <v>64</v>
       </c>
       <c r="C35" s="4">
         <f>(VlReg*Vn)/Vol_mea</f>
-        <v>21012.983266012696</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3" t="str">
         <f>DEC2HEX(C35,4)</f>
-        <v>5214</v>
+        <v>0000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
         <v>44</v>
       </c>
-      <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38">
-        <f>HEX2DEC("7a13")</f>
+      <c r="C38" s="3">
+        <f>HEX2DEC(D38)</f>
         <v>31251</v>
       </c>
-      <c r="D38" t="s">
-        <v>9</v>
+      <c r="D38" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39">
-        <f>HEX2DEC("6e49")/1000</f>
-        <v>28.233000000000001</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="C39" s="3">
+        <f>HEX2DEC(D39)/1000</f>
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40">
-        <v>0.65600000000000003</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
       <c r="C41" s="4">
         <f>(Cur_defL*C40)/Cur_meaL</f>
-        <v>726.12389756667733</v>
+        <v>31786.45327102804</v>
       </c>
       <c r="D41" s="3" t="str">
         <f>DEC2HEX(C41,4)</f>
-        <v>02D6</v>
+        <v>7C2A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="3">
+        <f>HEX2DEC(D44)</f>
+        <v>30000</v>
+      </c>
+      <c r="D44" s="6">
+        <v>7530</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="3">
+        <f>HEX2DEC(D45)/1000</f>
+        <v>30</v>
+      </c>
+      <c r="D45" s="5">
+        <v>7530</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="4">
+        <f>(Cur_defL*C46)/Cur_meaL</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="3" t="str">
+        <f>DEC2HEX(C47,4)</f>
+        <v>0000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>